<commit_message>
committo qui per NTT
</commit_message>
<xml_diff>
--- a/season/season-2324_csv.xlsx
+++ b/season/season-2324_csv.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="46">
   <si>
     <t>Giornata</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
   <si>
     <t>Empoli</t>
@@ -506,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E191"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -534,13 +537,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -551,10 +554,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -568,10 +571,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -585,16 +588,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -602,10 +605,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -619,13 +622,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -636,10 +639,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -653,13 +656,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -670,16 +673,16 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -687,13 +690,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -704,10 +707,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -721,16 +724,16 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -738,10 +741,10 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -755,10 +758,10 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -772,10 +775,10 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -789,10 +792,10 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -806,13 +809,13 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -823,16 +826,16 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -840,10 +843,10 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -857,13 +860,13 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -874,10 +877,10 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -891,10 +894,10 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -908,10 +911,10 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -925,16 +928,16 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -942,16 +945,16 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -959,10 +962,10 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
         <v>40</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -976,16 +979,16 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -993,16 +996,16 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1010,13 +1013,13 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
         <v>6</v>
@@ -1027,16 +1030,16 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1044,10 +1047,10 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -1061,10 +1064,10 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -1078,10 +1081,10 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
@@ -1095,16 +1098,16 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1112,10 +1115,10 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
@@ -1129,10 +1132,10 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
         <v>5</v>
@@ -1146,10 +1149,10 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -1163,16 +1166,16 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1180,13 +1183,13 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E40" t="s">
         <v>7</v>
@@ -1197,16 +1200,16 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1214,10 +1217,10 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
@@ -1231,16 +1234,16 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D43" t="s">
         <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1248,16 +1251,16 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
         <v>36</v>
       </c>
-      <c r="C44" t="s">
-        <v>35</v>
-      </c>
       <c r="D44" t="s">
         <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1265,10 +1268,10 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D45" t="s">
         <v>8</v>
@@ -1282,10 +1285,10 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
@@ -1299,13 +1302,13 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D47" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E47" t="s">
         <v>5</v>
@@ -1316,16 +1319,16 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" t="s">
         <v>43</v>
       </c>
-      <c r="C48" t="s">
-        <v>42</v>
-      </c>
       <c r="D48" t="s">
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1333,13 +1336,13 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E49" t="s">
         <v>6</v>
@@ -1350,16 +1353,16 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E50" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1367,10 +1370,10 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D51" t="s">
         <v>5</v>
@@ -1384,16 +1387,16 @@
         <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1401,10 +1404,10 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D53" t="s">
         <v>5</v>
@@ -1418,16 +1421,16 @@
         <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D54" t="s">
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1435,13 +1438,13 @@
         <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D55" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E55" t="s">
         <v>5</v>
@@ -1452,10 +1455,10 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -1469,16 +1472,16 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
       </c>
       <c r="E57" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1486,10 +1489,10 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D58" t="s">
         <v>8</v>
@@ -1503,10 +1506,10 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D59" t="s">
         <v>5</v>
@@ -1520,16 +1523,16 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" t="s">
         <v>34</v>
       </c>
-      <c r="C60" t="s">
-        <v>33</v>
-      </c>
       <c r="D60" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E60" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1537,10 +1540,10 @@
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D61" t="s">
         <v>8</v>
@@ -1554,13 +1557,13 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C62" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D62" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E62" t="s">
         <v>8</v>
@@ -1571,16 +1574,16 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1588,13 +1591,13 @@
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D64" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E64" t="s">
         <v>8</v>
@@ -1605,16 +1608,16 @@
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1622,10 +1625,10 @@
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C66" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
@@ -1639,16 +1642,16 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D67" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E67" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1656,16 +1659,16 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
       </c>
       <c r="E68" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1673,13 +1676,13 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C69" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D69" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E69" t="s">
         <v>5</v>
@@ -1690,16 +1693,16 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C70" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D70" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E70" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1707,16 +1710,16 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C71" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
       </c>
       <c r="E71" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1724,16 +1727,16 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C72" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D72" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E72" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1741,10 +1744,10 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
+        <v>31</v>
+      </c>
+      <c r="C73" t="s">
         <v>30</v>
-      </c>
-      <c r="C73" t="s">
-        <v>29</v>
       </c>
       <c r="D73" t="s">
         <v>5</v>
@@ -1758,10 +1761,10 @@
         <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C74" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D74" t="s">
         <v>6</v>
@@ -1775,16 +1778,16 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D75" t="s">
         <v>6</v>
       </c>
       <c r="E75" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1792,13 +1795,13 @@
         <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C76" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D76" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E76" t="s">
         <v>5</v>
@@ -1809,16 +1812,16 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C77" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D77" t="s">
         <v>7</v>
       </c>
       <c r="E77" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1826,10 +1829,10 @@
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C78" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D78" t="s">
         <v>6</v>
@@ -1843,10 +1846,10 @@
         <v>12</v>
       </c>
       <c r="B79" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C79" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -1860,10 +1863,10 @@
         <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C80" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D80" t="s">
         <v>5</v>
@@ -1877,10 +1880,10 @@
         <v>12</v>
       </c>
       <c r="B81" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C81" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D81" t="s">
         <v>5</v>
@@ -1894,10 +1897,10 @@
         <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C82" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D82" t="s">
         <v>5</v>
@@ -1911,13 +1914,13 @@
         <v>13</v>
       </c>
       <c r="B83" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D83" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E83" t="s">
         <v>7</v>
@@ -1928,13 +1931,13 @@
         <v>13</v>
       </c>
       <c r="B84" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C84" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D84" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E84" t="s">
         <v>6</v>
@@ -1945,16 +1948,16 @@
         <v>13</v>
       </c>
       <c r="B85" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C85" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D85" t="s">
         <v>5</v>
       </c>
       <c r="E85" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1962,10 +1965,10 @@
         <v>13</v>
       </c>
       <c r="B86" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C86" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
@@ -1979,10 +1982,10 @@
         <v>13</v>
       </c>
       <c r="B87" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C87" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
@@ -1996,16 +1999,16 @@
         <v>13</v>
       </c>
       <c r="B88" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C88" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
       </c>
       <c r="E88" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2013,13 +2016,13 @@
         <v>13</v>
       </c>
       <c r="B89" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C89" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D89" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E89" t="s">
         <v>5</v>
@@ -2030,10 +2033,10 @@
         <v>13</v>
       </c>
       <c r="B90" t="s">
+        <v>32</v>
+      </c>
+      <c r="C90" t="s">
         <v>31</v>
-      </c>
-      <c r="C90" t="s">
-        <v>30</v>
       </c>
       <c r="D90" t="s">
         <v>5</v>
@@ -2047,13 +2050,13 @@
         <v>13</v>
       </c>
       <c r="B91" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C91" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D91" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E91" t="s">
         <v>6</v>
@@ -2064,16 +2067,16 @@
         <v>14</v>
       </c>
       <c r="B92" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C92" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D92" t="s">
         <v>5</v>
       </c>
       <c r="E92" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2081,10 +2084,10 @@
         <v>14</v>
       </c>
       <c r="B93" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C93" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D93" t="s">
         <v>5</v>
@@ -2098,13 +2101,13 @@
         <v>14</v>
       </c>
       <c r="B94" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C94" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D94" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E94" t="s">
         <v>5</v>
@@ -2115,16 +2118,16 @@
         <v>14</v>
       </c>
       <c r="B95" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C95" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D95" t="s">
         <v>5</v>
       </c>
       <c r="E95" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2132,10 +2135,10 @@
         <v>14</v>
       </c>
       <c r="B96" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C96" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D96" t="s">
         <v>8</v>
@@ -2149,10 +2152,10 @@
         <v>14</v>
       </c>
       <c r="B97" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C97" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D97" t="s">
         <v>5</v>
@@ -2166,16 +2169,16 @@
         <v>14</v>
       </c>
       <c r="B98" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C98" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D98" t="s">
         <v>5</v>
       </c>
       <c r="E98" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2183,10 +2186,10 @@
         <v>14</v>
       </c>
       <c r="B99" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C99" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
@@ -2200,13 +2203,13 @@
         <v>14</v>
       </c>
       <c r="B100" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C100" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D100" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E100" t="s">
         <v>7</v>
@@ -2217,16 +2220,16 @@
         <v>14</v>
       </c>
       <c r="B101" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C101" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D101" t="s">
         <v>5</v>
       </c>
       <c r="E101" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2234,16 +2237,16 @@
         <v>15</v>
       </c>
       <c r="B102" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C102" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D102" t="s">
         <v>5</v>
       </c>
       <c r="E102" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2251,13 +2254,13 @@
         <v>15</v>
       </c>
       <c r="B103" t="s">
+        <v>42</v>
+      </c>
+      <c r="C103" t="s">
         <v>41</v>
       </c>
-      <c r="C103" t="s">
-        <v>40</v>
-      </c>
       <c r="D103" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E103" t="s">
         <v>6</v>
@@ -2268,10 +2271,10 @@
         <v>15</v>
       </c>
       <c r="B104" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C104" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D104" t="s">
         <v>5</v>
@@ -2285,13 +2288,13 @@
         <v>15</v>
       </c>
       <c r="B105" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C105" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D105" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E105" t="s">
         <v>5</v>
@@ -2302,10 +2305,10 @@
         <v>15</v>
       </c>
       <c r="B106" t="s">
+        <v>36</v>
+      </c>
+      <c r="C106" t="s">
         <v>35</v>
-      </c>
-      <c r="C106" t="s">
-        <v>34</v>
       </c>
       <c r="D106" t="s">
         <v>5</v>
@@ -2319,10 +2322,10 @@
         <v>15</v>
       </c>
       <c r="B107" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C107" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D107" t="s">
         <v>6</v>
@@ -2336,10 +2339,10 @@
         <v>15</v>
       </c>
       <c r="B108" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C108" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D108" t="s">
         <v>6</v>
@@ -2353,13 +2356,13 @@
         <v>15</v>
       </c>
       <c r="B109" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C109" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D109" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E109" t="s">
         <v>5</v>
@@ -2370,10 +2373,10 @@
         <v>15</v>
       </c>
       <c r="B110" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110" t="s">
         <v>25</v>
-      </c>
-      <c r="C110" t="s">
-        <v>24</v>
       </c>
       <c r="D110" t="s">
         <v>6</v>
@@ -2387,10 +2390,10 @@
         <v>15</v>
       </c>
       <c r="B111" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C111" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D111" t="s">
         <v>6</v>
@@ -2404,10 +2407,10 @@
         <v>16</v>
       </c>
       <c r="B112" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C112" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D112" t="s">
         <v>6</v>
@@ -2421,16 +2424,16 @@
         <v>16</v>
       </c>
       <c r="B113" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C113" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D113" t="s">
         <v>5</v>
       </c>
       <c r="E113" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2438,10 +2441,10 @@
         <v>16</v>
       </c>
       <c r="B114" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C114" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D114" t="s">
         <v>6</v>
@@ -2455,10 +2458,10 @@
         <v>16</v>
       </c>
       <c r="B115" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C115" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D115" t="s">
         <v>6</v>
@@ -2472,10 +2475,10 @@
         <v>16</v>
       </c>
       <c r="B116" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C116" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D116" t="s">
         <v>5</v>
@@ -2489,13 +2492,13 @@
         <v>16</v>
       </c>
       <c r="B117" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C117" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D117" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E117" t="s">
         <v>5</v>
@@ -2506,10 +2509,10 @@
         <v>16</v>
       </c>
       <c r="B118" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C118" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D118" t="s">
         <v>6</v>
@@ -2523,10 +2526,10 @@
         <v>16</v>
       </c>
       <c r="B119" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C119" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D119" t="s">
         <v>5</v>
@@ -2540,16 +2543,16 @@
         <v>16</v>
       </c>
       <c r="B120" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C120" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D120" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E120" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2557,16 +2560,16 @@
         <v>16</v>
       </c>
       <c r="B121" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C121" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D121" t="s">
         <v>6</v>
       </c>
       <c r="E121" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2574,10 +2577,10 @@
         <v>17</v>
       </c>
       <c r="B122" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C122" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D122" t="s">
         <v>6</v>
@@ -2591,10 +2594,10 @@
         <v>17</v>
       </c>
       <c r="B123" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C123" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D123" t="s">
         <v>5</v>
@@ -2608,16 +2611,16 @@
         <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C124" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D124" t="s">
         <v>5</v>
       </c>
       <c r="E124" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2625,10 +2628,10 @@
         <v>17</v>
       </c>
       <c r="B125" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C125" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D125" t="s">
         <v>5</v>
@@ -2642,10 +2645,10 @@
         <v>17</v>
       </c>
       <c r="B126" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C126" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D126" t="s">
         <v>7</v>
@@ -2659,10 +2662,10 @@
         <v>17</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C127" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D127" t="s">
         <v>6</v>
@@ -2676,10 +2679,10 @@
         <v>17</v>
       </c>
       <c r="B128" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C128" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D128" t="s">
         <v>7</v>
@@ -2693,10 +2696,10 @@
         <v>17</v>
       </c>
       <c r="B129" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C129" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D129" t="s">
         <v>5</v>
@@ -2710,10 +2713,10 @@
         <v>17</v>
       </c>
       <c r="B130" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C130" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D130" t="s">
         <v>6</v>
@@ -2727,16 +2730,16 @@
         <v>17</v>
       </c>
       <c r="B131" t="s">
+        <v>34</v>
+      </c>
+      <c r="C131" t="s">
         <v>33</v>
       </c>
-      <c r="C131" t="s">
-        <v>32</v>
-      </c>
       <c r="D131" t="s">
         <v>6</v>
       </c>
       <c r="E131" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -2744,10 +2747,10 @@
         <v>18</v>
       </c>
       <c r="B132" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C132" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D132" t="s">
         <v>5</v>
@@ -2761,10 +2764,10 @@
         <v>18</v>
       </c>
       <c r="B133" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C133" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D133" t="s">
         <v>5</v>
@@ -2778,16 +2781,16 @@
         <v>18</v>
       </c>
       <c r="B134" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C134" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D134" t="s">
         <v>5</v>
       </c>
       <c r="E134" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -2795,10 +2798,10 @@
         <v>18</v>
       </c>
       <c r="B135" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C135" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D135" t="s">
         <v>7</v>
@@ -2812,10 +2815,10 @@
         <v>18</v>
       </c>
       <c r="B136" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D136" t="s">
         <v>5</v>
@@ -2829,16 +2832,16 @@
         <v>18</v>
       </c>
       <c r="B137" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C137" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D137" t="s">
         <v>7</v>
       </c>
       <c r="E137" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -2846,10 +2849,10 @@
         <v>18</v>
       </c>
       <c r="B138" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C138" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D138" t="s">
         <v>7</v>
@@ -2863,10 +2866,10 @@
         <v>18</v>
       </c>
       <c r="B139" t="s">
+        <v>30</v>
+      </c>
+      <c r="C139" t="s">
         <v>29</v>
-      </c>
-      <c r="C139" t="s">
-        <v>28</v>
       </c>
       <c r="D139" t="s">
         <v>5</v>
@@ -2880,13 +2883,13 @@
         <v>18</v>
       </c>
       <c r="B140" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C140" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D140" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E140" t="s">
         <v>7</v>
@@ -2897,16 +2900,16 @@
         <v>18</v>
       </c>
       <c r="B141" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C141" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D141" t="s">
         <v>7</v>
       </c>
       <c r="E141" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -2914,16 +2917,16 @@
         <v>19</v>
       </c>
       <c r="B142" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C142" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D142" t="s">
         <v>5</v>
       </c>
       <c r="E142" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -2931,10 +2934,10 @@
         <v>19</v>
       </c>
       <c r="B143" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C143" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D143" t="s">
         <v>5</v>
@@ -2948,10 +2951,10 @@
         <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C144" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D144" t="s">
         <v>7</v>
@@ -2965,16 +2968,16 @@
         <v>19</v>
       </c>
       <c r="B145" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C145" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D145" t="s">
         <v>8</v>
       </c>
       <c r="E145" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -2982,16 +2985,16 @@
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C146" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D146" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E146" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -2999,16 +3002,16 @@
         <v>19</v>
       </c>
       <c r="B147" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C147" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D147" t="s">
         <v>5</v>
       </c>
       <c r="E147" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3016,10 +3019,10 @@
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C148" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D148" t="s">
         <v>5</v>
@@ -3033,10 +3036,10 @@
         <v>19</v>
       </c>
       <c r="B149" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C149" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D149" t="s">
         <v>5</v>
@@ -3050,10 +3053,10 @@
         <v>19</v>
       </c>
       <c r="B150" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C150" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D150" t="s">
         <v>5</v>
@@ -3067,10 +3070,10 @@
         <v>19</v>
       </c>
       <c r="B151" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C151" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D151" t="s">
         <v>6</v>
@@ -3084,10 +3087,10 @@
         <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C152" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D152" t="s">
         <v>5</v>
@@ -3101,10 +3104,10 @@
         <v>20</v>
       </c>
       <c r="B153" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C153" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D153" t="s">
         <v>6</v>
@@ -3118,10 +3121,10 @@
         <v>20</v>
       </c>
       <c r="B154" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C154" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D154" t="s">
         <v>6</v>
@@ -3135,16 +3138,16 @@
         <v>20</v>
       </c>
       <c r="B155" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C155" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D155" t="s">
         <v>5</v>
       </c>
       <c r="E155" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3152,16 +3155,16 @@
         <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C156" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D156" t="s">
         <v>7</v>
       </c>
       <c r="E156" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3169,16 +3172,16 @@
         <v>20</v>
       </c>
       <c r="B157" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C157" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D157" t="s">
         <v>5</v>
       </c>
       <c r="E157" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -3186,10 +3189,10 @@
         <v>20</v>
       </c>
       <c r="B158" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C158" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D158" t="s">
         <v>6</v>
@@ -3203,16 +3206,16 @@
         <v>20</v>
       </c>
       <c r="B159" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C159" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D159" t="s">
         <v>6</v>
       </c>
       <c r="E159" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3220,13 +3223,13 @@
         <v>20</v>
       </c>
       <c r="B160" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C160" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D160" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E160" t="s">
         <v>6</v>
@@ -3237,10 +3240,10 @@
         <v>20</v>
       </c>
       <c r="B161" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C161" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D161" t="s">
         <v>8</v>
@@ -3254,13 +3257,13 @@
         <v>21</v>
       </c>
       <c r="B162" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C162" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D162" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E162" t="s">
         <v>6</v>
@@ -3271,10 +3274,10 @@
         <v>21</v>
       </c>
       <c r="B163" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C163" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D163" t="s">
         <v>5</v>
@@ -3288,13 +3291,13 @@
         <v>21</v>
       </c>
       <c r="B164" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C164" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D164" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E164" t="s">
         <v>5</v>
@@ -3305,10 +3308,10 @@
         <v>21</v>
       </c>
       <c r="B165" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C165" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D165" t="s">
         <v>6</v>
@@ -3322,10 +3325,10 @@
         <v>21</v>
       </c>
       <c r="B166" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C166" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D166" t="s">
         <v>5</v>
@@ -3339,16 +3342,16 @@
         <v>21</v>
       </c>
       <c r="B167" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C167" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D167" t="s">
         <v>5</v>
       </c>
       <c r="E167" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3356,10 +3359,10 @@
         <v>21</v>
       </c>
       <c r="B168" t="s">
+        <v>33</v>
+      </c>
+      <c r="C168" t="s">
         <v>32</v>
-      </c>
-      <c r="C168" t="s">
-        <v>31</v>
       </c>
       <c r="D168" t="s">
         <v>5</v>
@@ -3373,16 +3376,16 @@
         <v>21</v>
       </c>
       <c r="B169" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C169" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D169" t="s">
         <v>6</v>
       </c>
       <c r="E169" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3390,16 +3393,16 @@
         <v>21</v>
       </c>
       <c r="B170" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C170" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D170" t="s">
         <v>6</v>
       </c>
       <c r="E170" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3407,16 +3410,16 @@
         <v>21</v>
       </c>
       <c r="B171" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C171" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D171" t="s">
         <v>6</v>
       </c>
       <c r="E171" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -3424,16 +3427,16 @@
         <v>22</v>
       </c>
       <c r="B172" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C172" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D172" t="s">
         <v>5</v>
       </c>
       <c r="E172" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -3441,16 +3444,16 @@
         <v>22</v>
       </c>
       <c r="B173" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C173" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D173" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E173" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -3458,10 +3461,10 @@
         <v>22</v>
       </c>
       <c r="B174" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C174" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D174" t="s">
         <v>5</v>
@@ -3475,10 +3478,10 @@
         <v>22</v>
       </c>
       <c r="B175" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C175" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D175" t="s">
         <v>7</v>
@@ -3492,16 +3495,16 @@
         <v>22</v>
       </c>
       <c r="B176" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C176" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D176" t="s">
         <v>5</v>
       </c>
       <c r="E176" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -3509,16 +3512,16 @@
         <v>22</v>
       </c>
       <c r="B177" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C177" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D177" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E177" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -3526,16 +3529,16 @@
         <v>22</v>
       </c>
       <c r="B178" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C178" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D178" t="s">
         <v>7</v>
       </c>
       <c r="E178" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -3543,13 +3546,13 @@
         <v>22</v>
       </c>
       <c r="B179" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C179" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D179" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E179" t="s">
         <v>5</v>
@@ -3560,16 +3563,16 @@
         <v>22</v>
       </c>
       <c r="B180" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C180" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D180" t="s">
         <v>5</v>
       </c>
       <c r="E180" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -3577,16 +3580,16 @@
         <v>22</v>
       </c>
       <c r="B181" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C181" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D181" t="s">
         <v>5</v>
       </c>
       <c r="E181" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -3594,10 +3597,10 @@
         <v>23</v>
       </c>
       <c r="B182" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C182" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D182" t="s">
         <v>5</v>
@@ -3611,10 +3614,10 @@
         <v>23</v>
       </c>
       <c r="B183" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C183" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D183" t="s">
         <v>6</v>
@@ -3628,10 +3631,10 @@
         <v>23</v>
       </c>
       <c r="B184" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C184" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D184" t="s">
         <v>6</v>
@@ -3645,10 +3648,10 @@
         <v>23</v>
       </c>
       <c r="B185" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C185" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D185" t="s">
         <v>5</v>
@@ -3662,16 +3665,16 @@
         <v>23</v>
       </c>
       <c r="B186" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C186" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D186" t="s">
         <v>5</v>
       </c>
       <c r="E186" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -3679,13 +3682,13 @@
         <v>23</v>
       </c>
       <c r="B187" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C187" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D187" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E187" t="s">
         <v>7</v>
@@ -3696,16 +3699,16 @@
         <v>23</v>
       </c>
       <c r="B188" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C188" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D188" t="s">
         <v>7</v>
       </c>
       <c r="E188" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -3713,10 +3716,10 @@
         <v>23</v>
       </c>
       <c r="B189" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C189" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D189" t="s">
         <v>5</v>
@@ -3730,10 +3733,10 @@
         <v>23</v>
       </c>
       <c r="B190" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C190" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D190" t="s">
         <v>5</v>
@@ -3747,16 +3750,84 @@
         <v>23</v>
       </c>
       <c r="B191" t="s">
+        <v>29</v>
+      </c>
+      <c r="C191" t="s">
+        <v>44</v>
+      </c>
+      <c r="D191" t="s">
+        <v>5</v>
+      </c>
+      <c r="E191" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" t="s">
+        <v>24</v>
+      </c>
+      <c r="B192" t="s">
+        <v>27</v>
+      </c>
+      <c r="C192" t="s">
+        <v>33</v>
+      </c>
+      <c r="D192" t="s">
+        <v>45</v>
+      </c>
+      <c r="E192" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" t="s">
+        <v>24</v>
+      </c>
+      <c r="B193" t="s">
+        <v>41</v>
+      </c>
+      <c r="C193" t="s">
+        <v>42</v>
+      </c>
+      <c r="D193" t="s">
+        <v>6</v>
+      </c>
+      <c r="E193" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" t="s">
+        <v>24</v>
+      </c>
+      <c r="B194" t="s">
+        <v>36</v>
+      </c>
+      <c r="C194" t="s">
+        <v>25</v>
+      </c>
+      <c r="D194" t="s">
+        <v>6</v>
+      </c>
+      <c r="E194" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" t="s">
+        <v>24</v>
+      </c>
+      <c r="B195" t="s">
+        <v>35</v>
+      </c>
+      <c r="C195" t="s">
         <v>28</v>
       </c>
-      <c r="C191" t="s">
-        <v>43</v>
-      </c>
-      <c r="D191" t="s">
-        <v>5</v>
-      </c>
-      <c r="E191" t="s">
-        <v>5</v>
+      <c r="D195" t="s">
+        <v>5</v>
+      </c>
+      <c r="E195" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>